<commit_message>
dl minor edits usda
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_DL.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_DL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdre/Documents/github/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DB7202-CE77-9940-85E2-11190BAD5460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C929F3-402F-BF4B-82BA-CBF2CB42AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37960" yWindow="7920" windowWidth="36640" windowHeight="12340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7820" windowWidth="30240" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="108">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -267,36 +267,15 @@
     <t>Na</t>
   </si>
   <si>
-    <t>90-120</t>
-  </si>
-  <si>
     <t>30+</t>
   </si>
   <si>
-    <t>1-5</t>
-  </si>
-  <si>
-    <t>120-190</t>
-  </si>
-  <si>
-    <t>30-156</t>
-  </si>
-  <si>
     <t>8+</t>
   </si>
   <si>
     <t>ailantifolia</t>
   </si>
   <si>
-    <t>50-80</t>
-  </si>
-  <si>
-    <t>30-60</t>
-  </si>
-  <si>
-    <t>15-40</t>
-  </si>
-  <si>
     <t>3+</t>
   </si>
   <si>
@@ -333,9 +312,6 @@
     <t>paper/pads</t>
   </si>
   <si>
-    <t>30-120</t>
-  </si>
-  <si>
     <t>western Oregon</t>
   </si>
   <si>
@@ -363,15 +339,6 @@
     <t>stored seeds</t>
   </si>
   <si>
-    <t>84-47</t>
-  </si>
-  <si>
-    <t>56-120</t>
-  </si>
-  <si>
-    <t>60-110</t>
-  </si>
-  <si>
     <t>high value reported before low value</t>
   </si>
   <si>
@@ -379,6 +346,45 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>warm_stratification_temp_C</t>
+  </si>
+  <si>
+    <t>cold_stratification_temp_C</t>
+  </si>
+  <si>
+    <t>30 to 120</t>
+  </si>
+  <si>
+    <t>84 to 47</t>
+  </si>
+  <si>
+    <t>56 to 120</t>
+  </si>
+  <si>
+    <t>60 to 110</t>
+  </si>
+  <si>
+    <t>90 to 120</t>
+  </si>
+  <si>
+    <t>120 to 190</t>
+  </si>
+  <si>
+    <t>30 to 156</t>
+  </si>
+  <si>
+    <t>1 to 5</t>
+  </si>
+  <si>
+    <t>50 to 80</t>
+  </si>
+  <si>
+    <t>30 to 60</t>
+  </si>
+  <si>
+    <t>15 to 40</t>
   </si>
 </sst>
 </file>
@@ -421,13 +427,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,16 +1003,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE19" sqref="AE19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,71 +1043,74 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+      <c r="J1" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="AD1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>604</v>
       </c>
@@ -1106,13 +1121,13 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
         <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>81</v>
       </c>
       <c r="G2">
         <v>14400</v>
@@ -1121,20 +1136,17 @@
         <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K2" t="s">
         <v>64</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
       <c r="N2" t="s">
         <v>64</v>
       </c>
@@ -1147,21 +1159,21 @@
       <c r="Q2" t="s">
         <v>64</v>
       </c>
-      <c r="R2">
+      <c r="R2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2">
         <v>42</v>
       </c>
-      <c r="S2" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2">
+      <c r="T2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2">
         <v>75</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>3</v>
       </c>
-      <c r="V2" t="s">
-        <v>64</v>
-      </c>
       <c r="W2" t="s">
         <v>64</v>
       </c>
@@ -1183,8 +1195,11 @@
       <c r="AC2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>604</v>
       </c>
@@ -1201,7 +1216,7 @@
         <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
         <v>64</v>
@@ -1213,20 +1228,17 @@
         <v>64</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
         <v>64</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>156</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>67</v>
       </c>
-      <c r="N3" t="s">
-        <v>64</v>
-      </c>
       <c r="O3" t="s">
         <v>64</v>
       </c>
@@ -1236,20 +1248,20 @@
       <c r="Q3" t="s">
         <v>64</v>
       </c>
-      <c r="R3">
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3">
         <v>30</v>
       </c>
-      <c r="S3" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3">
+      <c r="T3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3">
         <v>58</v>
       </c>
-      <c r="U3" t="s">
-        <v>78</v>
-      </c>
       <c r="V3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="W3" t="s">
         <v>64</v>
@@ -1272,8 +1284,11 @@
       <c r="AC3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>604</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>64</v>
@@ -1302,47 +1317,44 @@
         <v>64</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="L4" t="s">
-        <v>68</v>
-      </c>
       <c r="M4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N4">
+        <v>101</v>
+      </c>
+      <c r="N4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4">
         <v>30</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>20</v>
       </c>
-      <c r="P4" t="s">
-        <v>64</v>
-      </c>
       <c r="Q4" t="s">
         <v>64</v>
       </c>
       <c r="R4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T4">
+        <v>105</v>
+      </c>
+      <c r="T4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4">
         <v>65</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>7</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>54</v>
       </c>
-      <c r="W4" t="s">
-        <v>64</v>
-      </c>
       <c r="X4" t="s">
         <v>64</v>
       </c>
@@ -1358,11 +1370,14 @@
       <c r="AB4" t="s">
         <v>64</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD4">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>604</v>
       </c>
@@ -1379,7 +1394,7 @@
         <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>64</v>
@@ -1391,44 +1406,41 @@
         <v>64</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K5" t="s">
         <v>64</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>156</v>
       </c>
-      <c r="M5" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5">
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5">
         <v>30</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>20</v>
       </c>
-      <c r="P5" t="s">
-        <v>64</v>
-      </c>
       <c r="Q5" t="s">
         <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T5">
+        <v>68</v>
+      </c>
+      <c r="T5" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5">
         <v>41</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>4</v>
       </c>
-      <c r="V5" t="s">
-        <v>64</v>
-      </c>
       <c r="W5" t="s">
         <v>64</v>
       </c>
@@ -1450,8 +1462,11 @@
       <c r="AC5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>604</v>
       </c>
@@ -1468,7 +1483,7 @@
         <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>64</v>
@@ -1480,47 +1495,44 @@
         <v>64</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" t="s">
-        <v>71</v>
-      </c>
       <c r="M6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6">
+        <v>102</v>
+      </c>
+      <c r="N6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6">
         <v>30</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>20</v>
       </c>
-      <c r="P6" t="s">
-        <v>64</v>
-      </c>
       <c r="Q6" t="s">
         <v>64</v>
       </c>
-      <c r="R6">
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6">
         <v>49</v>
       </c>
-      <c r="S6" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6">
+      <c r="T6" t="s">
         <v>64</v>
       </c>
       <c r="U6">
+        <v>64</v>
+      </c>
+      <c r="V6">
         <v>5</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>10</v>
       </c>
-      <c r="W6" t="s">
-        <v>64</v>
-      </c>
       <c r="X6" t="s">
         <v>64</v>
       </c>
@@ -1536,11 +1548,14 @@
       <c r="AB6" t="s">
         <v>64</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD6">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>604</v>
       </c>
@@ -1557,7 +1572,7 @@
         <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>64</v>
@@ -1569,47 +1584,44 @@
         <v>64</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K7" t="s">
         <v>64</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>190</v>
       </c>
-      <c r="M7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N7">
+      <c r="N7" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7">
         <v>30</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>20</v>
       </c>
-      <c r="P7" t="s">
-        <v>64</v>
-      </c>
       <c r="Q7" t="s">
         <v>64</v>
       </c>
       <c r="R7" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
-      </c>
-      <c r="T7">
+        <v>106</v>
+      </c>
+      <c r="T7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7">
         <v>46</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>7</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>68</v>
       </c>
-      <c r="W7" t="s">
-        <v>64</v>
-      </c>
       <c r="X7" t="s">
         <v>64</v>
       </c>
@@ -1625,11 +1637,14 @@
       <c r="AB7" t="s">
         <v>64</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>604</v>
       </c>
@@ -1646,7 +1661,7 @@
         <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
         <v>64</v>
@@ -1658,47 +1673,44 @@
         <v>64</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K8" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" t="s">
-        <v>73</v>
-      </c>
-      <c r="N8">
+      <c r="M8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8">
         <v>30</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>20</v>
       </c>
-      <c r="P8" t="s">
-        <v>64</v>
-      </c>
       <c r="Q8" t="s">
         <v>64</v>
       </c>
       <c r="R8" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="S8" t="s">
-        <v>64</v>
-      </c>
-      <c r="T8">
+        <v>107</v>
+      </c>
+      <c r="T8" t="s">
+        <v>64</v>
+      </c>
+      <c r="U8">
         <v>50</v>
       </c>
-      <c r="U8" t="s">
-        <v>79</v>
-      </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>72</v>
+      </c>
+      <c r="W8">
         <v>60</v>
       </c>
-      <c r="W8" t="s">
-        <v>64</v>
-      </c>
       <c r="X8" t="s">
         <v>64</v>
       </c>
@@ -1714,11 +1726,14 @@
       <c r="AB8" t="s">
         <v>64</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD8">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>604</v>
       </c>
@@ -1735,7 +1750,7 @@
         <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
         <v>64</v>
@@ -1747,44 +1762,41 @@
         <v>64</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="K9" t="s">
         <v>64</v>
       </c>
-      <c r="L9" t="s">
-        <v>72</v>
-      </c>
       <c r="M9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9">
+        <v>103</v>
+      </c>
+      <c r="N9" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9">
         <v>30</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>20</v>
       </c>
-      <c r="P9" t="s">
-        <v>64</v>
-      </c>
       <c r="Q9" t="s">
         <v>64</v>
       </c>
-      <c r="R9">
+      <c r="R9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S9">
         <v>40</v>
       </c>
-      <c r="S9" t="s">
-        <v>64</v>
-      </c>
-      <c r="T9">
+      <c r="T9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9">
         <v>82</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>4</v>
       </c>
-      <c r="V9" t="s">
-        <v>64</v>
-      </c>
       <c r="W9" t="s">
         <v>64</v>
       </c>
@@ -1806,8 +1818,11 @@
       <c r="AC9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>554</v>
       </c>
@@ -1815,35 +1830,32 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10">
         <v>83</v>
       </c>
-      <c r="D10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10">
-        <v>83</v>
-      </c>
-      <c r="M10" t="s">
-        <v>64</v>
-      </c>
       <c r="N10" t="s">
         <v>64</v>
       </c>
@@ -1889,11 +1901,14 @@
       <c r="AB10" t="s">
         <v>64</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD10">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>554</v>
       </c>
@@ -1901,10 +1916,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
@@ -1927,42 +1942,39 @@
       <c r="K11" t="s">
         <v>64</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11">
+      <c r="N11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11">
         <v>30</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>20</v>
       </c>
-      <c r="P11" t="s">
-        <v>64</v>
-      </c>
       <c r="Q11" t="s">
         <v>64</v>
       </c>
-      <c r="R11">
+      <c r="R11" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11">
         <v>59</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>8</v>
       </c>
-      <c r="T11" t="s">
-        <v>64</v>
-      </c>
       <c r="U11" t="s">
         <v>64</v>
       </c>
-      <c r="V11">
+      <c r="V11" t="s">
+        <v>64</v>
+      </c>
+      <c r="W11">
         <v>7</v>
       </c>
-      <c r="W11" t="s">
-        <v>64</v>
-      </c>
       <c r="X11" t="s">
         <v>64</v>
       </c>
@@ -1978,14 +1990,17 @@
       <c r="AB11" t="s">
         <v>64</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD11">
         <v>213</v>
       </c>
-      <c r="AD11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>554</v>
       </c>
@@ -1993,10 +2008,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2019,42 +2034,39 @@
       <c r="K12" t="s">
         <v>64</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>60</v>
       </c>
-      <c r="M12" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12">
+      <c r="N12" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12">
         <v>30</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>20</v>
       </c>
-      <c r="P12" t="s">
-        <v>64</v>
-      </c>
       <c r="Q12" t="s">
         <v>64</v>
       </c>
-      <c r="R12">
+      <c r="R12" t="s">
+        <v>64</v>
+      </c>
+      <c r="S12">
         <v>15</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>16</v>
       </c>
-      <c r="T12" t="s">
-        <v>64</v>
-      </c>
       <c r="U12" t="s">
         <v>64</v>
       </c>
-      <c r="V12">
+      <c r="V12" t="s">
+        <v>64</v>
+      </c>
+      <c r="W12">
         <v>16</v>
       </c>
-      <c r="W12" t="s">
-        <v>64</v>
-      </c>
       <c r="X12" t="s">
         <v>64</v>
       </c>
@@ -2070,11 +2082,14 @@
       <c r="AB12" t="s">
         <v>64</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD12">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>554</v>
       </c>
@@ -2082,16 +2097,16 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
         <v>64</v>
@@ -2108,42 +2123,39 @@
       <c r="K13" t="s">
         <v>64</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0</v>
       </c>
-      <c r="M13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13">
+      <c r="N13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13">
         <v>30</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>20</v>
       </c>
-      <c r="P13" t="s">
-        <v>64</v>
-      </c>
       <c r="Q13" t="s">
         <v>64</v>
       </c>
-      <c r="R13">
+      <c r="R13" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13">
         <v>27</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>38</v>
       </c>
-      <c r="T13" t="s">
-        <v>64</v>
-      </c>
       <c r="U13" t="s">
         <v>64</v>
       </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>64</v>
+      </c>
+      <c r="W13">
         <v>28</v>
       </c>
-      <c r="W13" t="s">
-        <v>64</v>
-      </c>
       <c r="X13" t="s">
         <v>64</v>
       </c>
@@ -2159,11 +2171,14 @@
       <c r="AB13" t="s">
         <v>64</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD13">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>554</v>
       </c>
@@ -2171,16 +2186,16 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
@@ -2197,42 +2212,39 @@
       <c r="K14" t="s">
         <v>64</v>
       </c>
-      <c r="L14" t="s">
-        <v>90</v>
-      </c>
       <c r="M14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14">
+        <v>97</v>
+      </c>
+      <c r="N14" t="s">
+        <v>64</v>
+      </c>
+      <c r="O14">
         <v>30</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>20</v>
       </c>
-      <c r="P14" t="s">
-        <v>64</v>
-      </c>
       <c r="Q14" t="s">
         <v>64</v>
       </c>
-      <c r="R14">
+      <c r="R14" t="s">
+        <v>64</v>
+      </c>
+      <c r="S14">
         <v>37</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>31</v>
       </c>
-      <c r="T14" t="s">
-        <v>64</v>
-      </c>
       <c r="U14" t="s">
         <v>64</v>
       </c>
-      <c r="V14">
+      <c r="V14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W14">
         <v>26</v>
       </c>
-      <c r="W14" t="s">
-        <v>64</v>
-      </c>
       <c r="X14" t="s">
         <v>64</v>
       </c>
@@ -2248,11 +2260,14 @@
       <c r="AB14" t="s">
         <v>64</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD14">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>554</v>
       </c>
@@ -2260,16 +2275,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
         <v>64</v>
@@ -2286,42 +2301,39 @@
       <c r="K15" t="s">
         <v>64</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>0</v>
       </c>
-      <c r="M15" t="s">
-        <v>64</v>
-      </c>
-      <c r="N15">
-        <v>21</v>
+      <c r="N15" t="s">
+        <v>64</v>
       </c>
       <c r="O15">
         <v>21</v>
       </c>
-      <c r="P15" t="s">
-        <v>64</v>
+      <c r="P15">
+        <v>21</v>
       </c>
       <c r="Q15" t="s">
         <v>64</v>
       </c>
-      <c r="R15">
+      <c r="R15" t="s">
+        <v>64</v>
+      </c>
+      <c r="S15">
         <v>22</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>76</v>
       </c>
-      <c r="T15" t="s">
-        <v>64</v>
-      </c>
       <c r="U15" t="s">
         <v>64</v>
       </c>
-      <c r="V15">
+      <c r="V15" t="s">
+        <v>64</v>
+      </c>
+      <c r="W15">
         <v>74</v>
       </c>
-      <c r="W15" t="s">
-        <v>64</v>
-      </c>
       <c r="X15" t="s">
         <v>64</v>
       </c>
@@ -2337,11 +2349,14 @@
       <c r="AB15" t="s">
         <v>64</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD15">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>554</v>
       </c>
@@ -2349,16 +2364,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
@@ -2375,42 +2390,39 @@
       <c r="K16" t="s">
         <v>64</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>0</v>
       </c>
-      <c r="M16" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16">
+      <c r="N16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16">
         <v>21</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>16</v>
       </c>
-      <c r="P16" t="s">
-        <v>64</v>
-      </c>
       <c r="Q16" t="s">
         <v>64</v>
       </c>
-      <c r="R16">
+      <c r="R16" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16">
         <v>30</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>51</v>
       </c>
-      <c r="T16" t="s">
-        <v>64</v>
-      </c>
       <c r="U16" t="s">
         <v>64</v>
       </c>
-      <c r="V16">
+      <c r="V16" t="s">
+        <v>64</v>
+      </c>
+      <c r="W16">
         <v>42</v>
       </c>
-      <c r="W16" t="s">
-        <v>64</v>
-      </c>
       <c r="X16" t="s">
         <v>64</v>
       </c>
@@ -2426,11 +2438,14 @@
       <c r="AB16" t="s">
         <v>64</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD16">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>554</v>
       </c>
@@ -2438,16 +2453,16 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
@@ -2464,42 +2479,39 @@
       <c r="K17" t="s">
         <v>64</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17">
+      <c r="N17" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17">
         <v>16</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="P17" t="s">
-        <v>64</v>
-      </c>
       <c r="Q17" t="s">
         <v>64</v>
       </c>
-      <c r="R17">
+      <c r="R17" t="s">
+        <v>64</v>
+      </c>
+      <c r="S17">
         <v>30</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>51</v>
       </c>
-      <c r="T17" t="s">
-        <v>64</v>
-      </c>
       <c r="U17" t="s">
         <v>64</v>
       </c>
-      <c r="V17">
+      <c r="V17" t="s">
+        <v>64</v>
+      </c>
+      <c r="W17">
         <v>28</v>
       </c>
-      <c r="W17" t="s">
-        <v>64</v>
-      </c>
       <c r="X17" t="s">
         <v>64</v>
       </c>
@@ -2515,11 +2527,14 @@
       <c r="AB17" t="s">
         <v>64</v>
       </c>
-      <c r="AC17">
+      <c r="AC17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD17">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>554</v>
       </c>
@@ -2527,16 +2542,16 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>91</v>
-      </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
         <v>64</v>
@@ -2553,42 +2568,39 @@
       <c r="K18" t="s">
         <v>64</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>0</v>
       </c>
-      <c r="M18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N18">
+      <c r="N18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18">
         <v>10</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>4</v>
       </c>
-      <c r="P18" t="s">
-        <v>64</v>
-      </c>
       <c r="Q18" t="s">
         <v>64</v>
       </c>
-      <c r="R18">
+      <c r="R18" t="s">
+        <v>64</v>
+      </c>
+      <c r="S18">
         <v>30</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>41</v>
       </c>
-      <c r="T18" t="s">
-        <v>64</v>
-      </c>
       <c r="U18" t="s">
         <v>64</v>
       </c>
-      <c r="V18">
+      <c r="V18" t="s">
+        <v>64</v>
+      </c>
+      <c r="W18">
         <v>0</v>
       </c>
-      <c r="W18" t="s">
-        <v>64</v>
-      </c>
       <c r="X18" t="s">
         <v>64</v>
       </c>
@@ -2604,11 +2616,14 @@
       <c r="AB18" t="s">
         <v>64</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>554</v>
       </c>
@@ -2616,16 +2631,16 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" t="s">
-        <v>91</v>
-      </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
@@ -2642,42 +2657,39 @@
       <c r="K19" t="s">
         <v>64</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>60</v>
       </c>
-      <c r="M19" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19">
+      <c r="N19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19">
         <v>21</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>16</v>
       </c>
-      <c r="P19" t="s">
-        <v>64</v>
-      </c>
       <c r="Q19" t="s">
         <v>64</v>
       </c>
-      <c r="R19">
+      <c r="R19" t="s">
+        <v>64</v>
+      </c>
+      <c r="S19">
         <v>30</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>45</v>
       </c>
-      <c r="T19" t="s">
-        <v>64</v>
-      </c>
       <c r="U19" t="s">
         <v>64</v>
       </c>
-      <c r="V19">
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19">
         <v>39</v>
       </c>
-      <c r="W19" t="s">
-        <v>64</v>
-      </c>
       <c r="X19" t="s">
         <v>64</v>
       </c>
@@ -2693,11 +2705,14 @@
       <c r="AB19" t="s">
         <v>64</v>
       </c>
-      <c r="AC19">
+      <c r="AC19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD19">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>554</v>
       </c>
@@ -2705,16 +2720,16 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>91</v>
-      </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
         <v>64</v>
@@ -2731,42 +2746,39 @@
       <c r="K20" t="s">
         <v>64</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>60</v>
       </c>
-      <c r="M20" t="s">
-        <v>64</v>
-      </c>
-      <c r="N20">
+      <c r="N20" t="s">
+        <v>64</v>
+      </c>
+      <c r="O20">
         <v>16</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>10</v>
       </c>
-      <c r="P20" t="s">
-        <v>64</v>
-      </c>
       <c r="Q20" t="s">
         <v>64</v>
       </c>
-      <c r="R20">
+      <c r="R20" t="s">
+        <v>64</v>
+      </c>
+      <c r="S20">
         <v>30</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>40</v>
       </c>
-      <c r="T20" t="s">
-        <v>64</v>
-      </c>
       <c r="U20" t="s">
         <v>64</v>
       </c>
-      <c r="V20">
+      <c r="V20" t="s">
+        <v>64</v>
+      </c>
+      <c r="W20">
         <v>31</v>
       </c>
-      <c r="W20" t="s">
-        <v>64</v>
-      </c>
       <c r="X20" t="s">
         <v>64</v>
       </c>
@@ -2782,11 +2794,14 @@
       <c r="AB20" t="s">
         <v>64</v>
       </c>
-      <c r="AC20">
+      <c r="AC20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD20">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>554</v>
       </c>
@@ -2794,16 +2809,16 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
         <v>64</v>
@@ -2820,42 +2835,39 @@
       <c r="K21" t="s">
         <v>64</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>60</v>
       </c>
-      <c r="M21" t="s">
-        <v>64</v>
-      </c>
-      <c r="N21">
+      <c r="N21" t="s">
+        <v>64</v>
+      </c>
+      <c r="O21">
         <v>10</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>4</v>
       </c>
-      <c r="P21" t="s">
-        <v>64</v>
-      </c>
       <c r="Q21" t="s">
         <v>64</v>
       </c>
-      <c r="R21">
+      <c r="R21" t="s">
+        <v>64</v>
+      </c>
+      <c r="S21">
         <v>30</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>50</v>
       </c>
-      <c r="T21" t="s">
-        <v>64</v>
-      </c>
       <c r="U21" t="s">
         <v>64</v>
       </c>
-      <c r="V21">
+      <c r="V21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W21">
         <v>23</v>
       </c>
-      <c r="W21" t="s">
-        <v>64</v>
-      </c>
       <c r="X21" t="s">
         <v>64</v>
       </c>
@@ -2871,11 +2883,14 @@
       <c r="AB21" t="s">
         <v>64</v>
       </c>
-      <c r="AC21">
+      <c r="AC21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD21">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>554</v>
       </c>
@@ -2883,16 +2898,16 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
         <v>83</v>
       </c>
-      <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>91</v>
-      </c>
       <c r="F22" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
         <v>64</v>
@@ -2909,42 +2924,39 @@
       <c r="K22" t="s">
         <v>64</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>150</v>
       </c>
-      <c r="M22" t="s">
-        <v>64</v>
-      </c>
-      <c r="N22">
+      <c r="N22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O22">
         <v>21</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>16</v>
       </c>
-      <c r="P22" t="s">
-        <v>64</v>
-      </c>
       <c r="Q22" t="s">
         <v>64</v>
       </c>
-      <c r="R22">
+      <c r="R22" t="s">
+        <v>64</v>
+      </c>
+      <c r="S22">
         <v>30</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>59</v>
       </c>
-      <c r="T22" t="s">
-        <v>64</v>
-      </c>
       <c r="U22" t="s">
         <v>64</v>
       </c>
-      <c r="V22">
+      <c r="V22" t="s">
+        <v>64</v>
+      </c>
+      <c r="W22">
         <v>55</v>
       </c>
-      <c r="W22" t="s">
-        <v>64</v>
-      </c>
       <c r="X22" t="s">
         <v>64</v>
       </c>
@@ -2960,11 +2972,14 @@
       <c r="AB22" t="s">
         <v>64</v>
       </c>
-      <c r="AC22">
+      <c r="AC22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>554</v>
       </c>
@@ -2972,16 +2987,16 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s">
         <v>64</v>
@@ -2998,42 +3013,39 @@
       <c r="K23" t="s">
         <v>64</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>150</v>
       </c>
-      <c r="M23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N23">
+      <c r="N23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O23">
         <v>10</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>4</v>
       </c>
-      <c r="P23" t="s">
-        <v>64</v>
-      </c>
       <c r="Q23" t="s">
         <v>64</v>
       </c>
-      <c r="R23">
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23">
         <v>30</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>40</v>
       </c>
-      <c r="T23" t="s">
-        <v>64</v>
-      </c>
       <c r="U23" t="s">
         <v>64</v>
       </c>
-      <c r="V23">
+      <c r="V23" t="s">
+        <v>64</v>
+      </c>
+      <c r="W23">
         <v>32</v>
       </c>
-      <c r="W23" t="s">
-        <v>64</v>
-      </c>
       <c r="X23" t="s">
         <v>64</v>
       </c>
@@ -3049,11 +3061,14 @@
       <c r="AB23" t="s">
         <v>64</v>
       </c>
-      <c r="AC23">
+      <c r="AC23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD23">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>523</v>
       </c>
@@ -3061,10 +3076,10 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
         <v>64</v>
@@ -3087,21 +3102,18 @@
       <c r="K24" t="s">
         <v>64</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>90</v>
       </c>
-      <c r="M24" t="s">
-        <v>64</v>
-      </c>
-      <c r="N24">
+      <c r="N24" t="s">
+        <v>64</v>
+      </c>
+      <c r="O24">
         <v>30</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>20</v>
       </c>
-      <c r="P24" t="s">
-        <v>64</v>
-      </c>
       <c r="Q24" t="s">
         <v>64</v>
       </c>
@@ -3118,10 +3130,10 @@
         <v>64</v>
       </c>
       <c r="V24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="W24" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="X24" t="s">
         <v>64</v>
@@ -3138,11 +3150,14 @@
       <c r="AB24" t="s">
         <v>64</v>
       </c>
-      <c r="AC24">
+      <c r="AC24" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD24">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>523</v>
       </c>
@@ -3150,16 +3165,16 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
         <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
         <v>64</v>
@@ -3176,33 +3191,30 @@
       <c r="K25" t="s">
         <v>64</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>42</v>
       </c>
-      <c r="M25" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25">
+      <c r="N25" t="s">
+        <v>64</v>
+      </c>
+      <c r="O25">
         <v>30</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>20</v>
       </c>
-      <c r="P25" t="s">
-        <v>64</v>
-      </c>
       <c r="Q25" t="s">
         <v>64</v>
       </c>
       <c r="R25" t="s">
         <v>64</v>
       </c>
-      <c r="S25">
+      <c r="S25" t="s">
+        <v>64</v>
+      </c>
+      <c r="T25">
         <v>81</v>
       </c>
-      <c r="T25" t="s">
-        <v>64</v>
-      </c>
       <c r="U25" t="s">
         <v>64</v>
       </c>
@@ -3231,10 +3243,13 @@
         <v>64</v>
       </c>
       <c r="AD25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>523</v>
       </c>
@@ -3242,16 +3257,16 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
         <v>64</v>
@@ -3260,7 +3275,7 @@
         <v>64</v>
       </c>
       <c r="I26" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J26" t="s">
         <v>64</v>
@@ -3268,20 +3283,17 @@
       <c r="K26" t="s">
         <v>64</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>140</v>
       </c>
-      <c r="M26" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
+      <c r="N26" t="s">
+        <v>64</v>
       </c>
       <c r="O26">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
-        <v>64</v>
+      <c r="P26">
+        <v>1</v>
       </c>
       <c r="Q26" t="s">
         <v>64</v>
@@ -3299,10 +3311,10 @@
         <v>64</v>
       </c>
       <c r="V26" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="W26" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="X26" t="s">
         <v>64</v>
@@ -3319,11 +3331,14 @@
       <c r="AB26" t="s">
         <v>64</v>
       </c>
-      <c r="AC26">
+      <c r="AC26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD26">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>523</v>
       </c>
@@ -3331,16 +3346,16 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
         <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
         <v>64</v>
@@ -3349,7 +3364,7 @@
         <v>64</v>
       </c>
       <c r="I27" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J27" t="s">
         <v>64</v>
@@ -3357,20 +3372,17 @@
       <c r="K27" t="s">
         <v>64</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>150</v>
       </c>
-      <c r="M27" t="s">
-        <v>64</v>
-      </c>
-      <c r="N27">
-        <v>5</v>
+      <c r="N27" t="s">
+        <v>64</v>
       </c>
       <c r="O27">
         <v>5</v>
       </c>
-      <c r="P27" t="s">
-        <v>64</v>
+      <c r="P27">
+        <v>5</v>
       </c>
       <c r="Q27" t="s">
         <v>64</v>
@@ -3388,10 +3400,10 @@
         <v>64</v>
       </c>
       <c r="V27" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="W27" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="X27" t="s">
         <v>64</v>
@@ -3408,11 +3420,14 @@
       <c r="AB27" t="s">
         <v>64</v>
       </c>
-      <c r="AC27">
+      <c r="AC27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD27">
         <v>100</v>
       </c>
-      <c r="AD27" t="s">
-        <v>104</v>
+      <c r="AE27" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>